<commit_message>
Did some formating in Details file
</commit_message>
<xml_diff>
--- a/Details.xlsx
+++ b/Details.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29029"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sujit Singh\Desktop\BharatSpiceWorld\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A6FBA8-E0E0-4654-8D6F-98159F37B878}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65CE570-71E9-496A-894C-094CE8B1280A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{AE1EE7FA-8155-4B77-AA66-490FF771BDBA}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="51">
   <si>
     <t>Seller</t>
   </si>
@@ -186,13 +186,16 @@
   </si>
   <si>
     <t>Seller pack good and through carrier put goods beside ship and from here risk and cost gets transferred to Buyer, Insurance is negotiable</t>
+  </si>
+  <si>
+    <t>Terms</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,8 +211,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -240,6 +251,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -263,14 +292,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 2" xfId="1" builtinId="17"/>
@@ -606,219 +641,213 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFDECF7F-3D9E-40F7-8057-DB1902A19EF2}">
-  <dimension ref="A1:O13"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="8.7265625" customWidth="1"/>
-    <col min="7" max="7" width="6.7265625" customWidth="1"/>
-    <col min="9" max="9" width="24.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="145.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7265625" customWidth="1"/>
+    <col min="5" max="5" width="24.36328125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="145.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
-      <c r="N1" s="1"/>
-      <c r="O1" s="1"/>
-    </row>
-    <row r="2" spans="1:15" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="D2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
+    <row r="3" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A3" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="D3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
+    <row r="4" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="2" t="s">
+      <c r="D4" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="F4" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
+    <row r="5" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A5" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H5" s="2" t="s">
+      <c r="D5" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="F5" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
+    <row r="6" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A6" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="2" t="s">
+      <c r="D6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="I6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="F6" s="3" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
+    <row r="7" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="H7" s="2" t="s">
+      <c r="D7" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="F7" s="3" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
+    <row r="8" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A8" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="H8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="J8" s="4" t="s">
+      <c r="F8" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
+    <row r="9" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A9" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="H9" s="2" t="s">
+      <c r="D9" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="I9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="J9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
+    <row r="10" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A10" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="H10" s="2" t="s">
+      <c r="D10" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I10" s="3" t="s">
+      <c r="E10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="J10" s="4" t="s">
+      <c r="F10" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="H11" s="2" t="s">
+    <row r="11" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="D11" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="E11" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="F11" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="H12" s="2" t="s">
+    <row r="12" spans="1:6" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="D12" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="I12" s="3" t="s">
+      <c r="E12" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="J12" s="4" t="s">
+      <c r="F12" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="13" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:O1"/>
+  <mergeCells count="2">
+    <mergeCell ref="D1:F1"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>